<commit_message>
Added family history of diabetes, deleted cca analysis results.
</commit_message>
<xml_diff>
--- a/data/Phenotypes Variable List.xlsx
+++ b/data/Phenotypes Variable List.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7428B96C-3208-4CE3-81F5-4B2432E13234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482A199F-9500-49D8-8964-7AE0D0E628C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Harmonized" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3434" uniqueCount="2259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3473" uniqueCount="2295">
   <si>
     <t>harmonized</t>
   </si>
@@ -7201,12 +7201,120 @@
   <si>
     <t>drseveritysubject</t>
   </si>
+  <si>
+    <t>While the participant’s mother was pregnant with the participant, did a health care provider ever tell her that she had diabetes?</t>
+  </si>
+  <si>
+    <t>MOMGDM</t>
+  </si>
+  <si>
+    <t>If YES, a. Did the diabetes go away after the participant was born?</t>
+  </si>
+  <si>
+    <t>MOMGDMA</t>
+  </si>
+  <si>
+    <t>Did the participant’s mother have diabetes with any other pregnancy?</t>
+  </si>
+  <si>
+    <t>MGDMOTH</t>
+  </si>
+  <si>
+    <t>Was the participant’s mother ever diagnosed with diabetes?</t>
+  </si>
+  <si>
+    <t>MOMDBNOW</t>
+  </si>
+  <si>
+    <t>Was the participant’s father ever diagnosed with diabetes?</t>
+  </si>
+  <si>
+    <t>DADDBNOW</t>
+  </si>
+  <si>
+    <t>Has a full sibling with history of diabetes?</t>
+  </si>
+  <si>
+    <t>FULLDIAB</t>
+  </si>
+  <si>
+    <t>Has a half sibling with history of diabetes?</t>
+  </si>
+  <si>
+    <t>HALFDIAB</t>
+  </si>
+  <si>
+    <t>mom_gdm</t>
+  </si>
+  <si>
+    <t>mom_gdma</t>
+  </si>
+  <si>
+    <t>mom_gdmoth</t>
+  </si>
+  <si>
+    <t>mom_dm</t>
+  </si>
+  <si>
+    <t>dad_dm</t>
+  </si>
+  <si>
+    <t>fullsib_dm</t>
+  </si>
+  <si>
+    <t>halfsib_dm</t>
+  </si>
+  <si>
+    <t>Did biologic grandparent ever have diabetes?</t>
+  </si>
+  <si>
+    <t>GRANDIAB</t>
+  </si>
+  <si>
+    <t>grand_dm</t>
+  </si>
+  <si>
+    <t>motherdiab</t>
+  </si>
+  <si>
+    <t>Did your child's biological mother have any form of diabetes when she was pregnant with the child? This includes Type 1 diabetes, Type 2 diabetes, gestational diabetes, or other type of diabetes.</t>
+  </si>
+  <si>
+    <t>mothpregdiab</t>
+  </si>
+  <si>
+    <t>Does your child's biological father have diabetes?</t>
+  </si>
+  <si>
+    <t>fatherdiab</t>
+  </si>
+  <si>
+    <t>How many full or half brothers have diabetes?</t>
+  </si>
+  <si>
+    <t>brotherdiab</t>
+  </si>
+  <si>
+    <t>bro_dm</t>
+  </si>
+  <si>
+    <t>How many full or half sisters have diabetes?</t>
+  </si>
+  <si>
+    <t>sis_dm</t>
+  </si>
+  <si>
+    <t>sisterdiab</t>
+  </si>
+  <si>
+    <t>Does your child's biological mother have diabetes?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -7342,8 +7450,14 @@
       <color theme="1"/>
       <name val="ArialMT"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7383,18 +7497,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -7448,14 +7550,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -9431,1857 +9531,1858 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0165A7-F003-446B-8586-D5FFFC81746F}">
-  <dimension ref="A1:D163"/>
+  <dimension ref="A1:D168"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C152" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C150" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B154" sqref="B154"/>
+      <selection pane="bottomRight" activeCell="B170" sqref="B170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="69.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.1796875" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="69.453125" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1796875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="28" t="s">
         <v>492</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="28" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A2,Harmonized!A:A,0))</f>
         <v>id</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="A3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A3,Harmonized!A:A,0))</f>
         <v>study_id</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="28" t="s">
         <v>407</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="28" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="A4" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A4,Harmonized!A:A,0))</f>
         <v>dmduration</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="28" t="s">
         <v>429</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="28" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="A5" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A5,Harmonized!A:A,0))</f>
         <v>dmagediag</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="28" t="s">
         <v>428</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="28" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="A6" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B6" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A6,Harmonized!A:A,0))</f>
         <v>age</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="28" t="s">
         <v>430</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="28" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="A7" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B7" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A7,Harmonized!A:A,0))</f>
         <v>female</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="28" t="s">
         <v>431</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="28" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" t="s">
+      <c r="A8" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B8" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A8,Harmonized!A:A,0))</f>
         <v>race</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="28" t="s">
         <v>418</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="28" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" t="s">
+      <c r="A9" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A9,Harmonized!A:A,0))</f>
         <v>ethnicity</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" t="s">
+      <c r="A10" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="B10" t="str">
+      <c r="B10" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A10,Harmonized!A:A,0))</f>
         <v>alcohol</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="A11" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="3" t="str">
+      <c r="B11" s="30" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A11,Harmonized!A:A,0))</f>
         <v>smoking</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="28" t="s">
         <v>495</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" t="s">
+      <c r="A12" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B12" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A12,Harmonized!A:A,0))</f>
         <v>dmfamilyhistory</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="28" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" t="s">
+      <c r="A13" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B13" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A13,Harmonized!A:A,0))</f>
         <v>height</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="28" t="s">
         <v>367</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="28" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" t="s">
+      <c r="A14" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B14" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A14,Harmonized!A:A,0))</f>
         <v>weight</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="28" t="s">
         <v>303</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="28" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" t="s">
+      <c r="A15" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="str">
+      <c r="B15" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A15,Harmonized!A:A,0))</f>
         <v>bmi</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="28" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" t="s">
+      <c r="A16" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B16" t="str">
+      <c r="B16" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A16,Harmonized!A:A,0))</f>
         <v>sbp</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="28" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" t="s">
+      <c r="A17" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B17" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A17,Harmonized!A:A,0))</f>
         <v>dbp</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="28" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" t="s">
+      <c r="A18" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B18" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A18,Harmonized!A:A,0))</f>
         <v>wc</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="28" t="s">
         <v>432</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="28" t="s">
         <v>545</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" t="s">
+      <c r="A19" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B19" t="str">
+      <c r="B19" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A19,Harmonized!A:A,0))</f>
         <v>hba1c</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="28" t="s">
         <v>464</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="28" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" t="s">
+      <c r="A20" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B20" t="str">
+      <c r="B20" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A20,Harmonized!A:A,0))</f>
         <v>insulinf</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" t="s">
+      <c r="A21" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B21" t="str">
+      <c r="B21" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A21,Harmonized!A:A,0))</f>
         <v>cpeptidef</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="28" t="s">
         <v>474</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="28" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" t="s">
+      <c r="A22" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B22" t="str">
+      <c r="B22" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A22,Harmonized!A:A,0))</f>
         <v>glucosef</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="28" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" t="s">
+      <c r="A23" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B23" t="str">
+      <c r="B23" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A23,Harmonized!A:A,0))</f>
         <v>glucoser</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" t="s">
+      <c r="A24" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B24" t="str">
+      <c r="B24" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A24,Harmonized!A:A,0))</f>
         <v>glucose2h</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" t="s">
+      <c r="A25" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B25" t="str">
+      <c r="B25" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A25,Harmonized!A:A,0))</f>
         <v>homab</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" t="s">
+      <c r="A26" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B26" t="str">
+      <c r="B26" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A26,Harmonized!A:A,0))</f>
         <v>homair</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" t="s">
+      <c r="A27" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="B27" t="str">
+      <c r="B27" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A27,Harmonized!A:A,0))</f>
         <v>totalc</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="28" t="s">
         <v>465</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="28" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" t="s">
+      <c r="A28" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B28" t="str">
+      <c r="B28" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A28,Harmonized!A:A,0))</f>
         <v>ldlc</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="28" t="s">
         <v>466</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="28" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" t="s">
+      <c r="A29" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B29" t="str">
+      <c r="B29" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A29,Harmonized!A:A,0))</f>
         <v>hdlc</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="28" t="s">
         <v>467</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="28" t="s">
         <v>540</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" t="s">
+      <c r="A30" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B30" t="str">
+      <c r="B30" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A30,Harmonized!A:A,0))</f>
         <v>vldlc</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="28" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" t="s">
+      <c r="A31" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="B31" t="str">
+      <c r="B31" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A31,Harmonized!A:A,0))</f>
         <v>tgl</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="28" t="s">
         <v>541</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" t="s">
+      <c r="A32" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B32" t="str">
+      <c r="B32" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A32,Harmonized!A:A,0))</f>
         <v>serumcreatinine</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="28" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" t="s">
+      <c r="A33" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B33" t="str">
+      <c r="B33" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A33,Harmonized!A:A,0))</f>
         <v>urinealbumin</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="28" t="s">
         <v>468</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="28" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" t="s">
+      <c r="A34" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B34" t="str">
+      <c r="B34" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A34,Harmonized!A:A,0))</f>
         <v>urinecreatinine</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="28" t="s">
         <v>469</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="28" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" t="s">
+      <c r="A35" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="B35" t="str">
+      <c r="B35" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A35,Harmonized!A:A,0))</f>
         <v>uacr</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="28" t="s">
         <v>470</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="28" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" t="s">
+      <c r="A36" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B36" t="str">
+      <c r="B36" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A36,Harmonized!A:A,0))</f>
         <v>egfr</v>
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" t="s">
+      <c r="A37" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="B37" t="str">
+      <c r="B37" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A37,Harmonized!A:A,0))</f>
         <v>ast</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" t="s">
+      <c r="A38" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="B38" t="str">
+      <c r="B38" s="28" t="str">
         <f>INDEX(Harmonized!B:B,MATCH(A38,Harmonized!A:A,0))</f>
         <v>alt</v>
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="31" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" t="s">
+      <c r="A41" s="28" t="s">
         <v>409</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="28" t="s">
         <v>410</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="28" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" t="s">
+      <c r="A42" s="28" t="s">
         <v>412</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="28" t="s">
         <v>413</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="28" t="s">
         <v>414</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="28" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" t="s">
+      <c r="A43" s="28" t="s">
         <v>415</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="28" t="s">
         <v>416</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="28" t="s">
         <v>417</v>
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44" t="s">
+      <c r="A44" s="28" t="s">
         <v>420</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="28" t="s">
         <v>421</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="28" t="s">
         <v>419</v>
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45" t="s">
+      <c r="A45" s="28" t="s">
         <v>422</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="28" t="s">
         <v>423</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="28" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46" t="s">
+      <c r="A46" s="28" t="s">
         <v>425</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="28" t="s">
         <v>426</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="28" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" t="s">
+      <c r="A47" s="28" t="s">
         <v>437</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="28" t="s">
         <v>441</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="28" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" t="s">
+      <c r="A48" s="28" t="s">
         <v>438</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="28" t="s">
         <v>442</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="28" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" t="s">
+      <c r="A49" s="28" t="s">
         <v>439</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="28" t="s">
         <v>443</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="28" t="s">
         <v>435</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" t="s">
+      <c r="A50" s="28" t="s">
         <v>440</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="28" t="s">
         <v>444</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="28" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" t="s">
+      <c r="A51" s="28" t="s">
         <v>446</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="28" t="s">
         <v>450</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="28" t="s">
         <v>448</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="28" t="s">
         <v>869</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" t="s">
+      <c r="A52" s="28" t="s">
         <v>447</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="28" t="s">
         <v>451</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="28" t="s">
         <v>449</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="28" t="s">
         <v>494</v>
       </c>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" t="s">
+      <c r="A53" s="28" t="s">
         <v>452</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="28" t="s">
         <v>460</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="28" t="s">
         <v>456</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="28" t="s">
         <v>886</v>
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" t="s">
+      <c r="A54" s="28" t="s">
         <v>453</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="28" t="s">
         <v>461</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="28" t="s">
         <v>457</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="28" t="s">
         <v>887</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" t="s">
+      <c r="A55" s="28" t="s">
         <v>454</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="28" t="s">
         <v>462</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="28" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" t="s">
+      <c r="A56" s="28" t="s">
         <v>455</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="28" t="s">
         <v>463</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="28" t="s">
         <v>459</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="28" t="s">
         <v>493</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" t="s">
+      <c r="A57" s="28" t="s">
         <v>471</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="28" t="s">
         <v>473</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="28" t="s">
         <v>472</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="28" t="s">
         <v>472</v>
       </c>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" t="s">
+      <c r="A58" s="28" t="s">
         <v>480</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="28" t="s">
         <v>486</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="28" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" t="s">
+      <c r="A59" s="28" t="s">
         <v>477</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="28" t="s">
         <v>487</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="28" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" t="s">
+      <c r="A60" s="28" t="s">
         <v>479</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="28" t="s">
         <v>488</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="28" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" t="s">
+      <c r="A61" s="28" t="s">
         <v>478</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="28" t="s">
         <v>489</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="28" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" t="s">
+      <c r="A62" s="28" t="s">
         <v>484</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="28" t="s">
         <v>490</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="28" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" t="s">
+      <c r="A63" s="28" t="s">
         <v>497</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="28" t="s">
         <v>634</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="28" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" t="s">
+      <c r="A64" s="28" t="s">
         <v>498</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="28" t="s">
         <v>635</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="28" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" t="s">
+      <c r="A65" s="28" t="s">
         <v>499</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="28" t="s">
         <v>637</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="28" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" t="s">
+      <c r="A66" s="28" t="s">
         <v>500</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="28" t="s">
         <v>638</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="28" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" t="s">
+      <c r="A67" s="28" t="s">
         <v>501</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="28" t="s">
         <v>639</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="28" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" t="s">
+      <c r="A68" s="28" t="s">
         <v>502</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="28" t="s">
         <v>636</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="28" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" t="s">
+      <c r="A69" s="28" t="s">
         <v>503</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="28" t="s">
         <v>640</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="28" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" t="s">
+      <c r="A70" s="28" t="s">
         <v>519</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="28" t="s">
         <v>641</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="28" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" t="s">
+      <c r="A71" s="28" t="s">
         <v>520</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="28" t="s">
         <v>642</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="28" t="s">
         <v>511</v>
       </c>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" t="s">
+      <c r="A72" s="28" t="s">
         <v>521</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="28" t="s">
         <v>643</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="28" t="s">
         <v>512</v>
       </c>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" t="s">
+      <c r="A73" s="28" t="s">
         <v>522</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="28" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" t="s">
+      <c r="A74" s="28" t="s">
         <v>523</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="28" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" t="s">
+      <c r="A75" s="28" t="s">
         <v>524</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="28" t="s">
         <v>644</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="28" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" t="s">
+      <c r="A76" s="28" t="s">
         <v>525</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="28" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" t="s">
+      <c r="A77" s="28" t="s">
         <v>526</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="28" t="s">
         <v>517</v>
       </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" t="s">
+      <c r="A78" s="28" t="s">
         <v>527</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="28" t="s">
         <v>645</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="28" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" t="s">
+      <c r="A79" s="28" t="s">
         <v>531</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="28" t="s">
         <v>528</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D79" s="28" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" t="s">
+      <c r="A80" s="28" t="s">
         <v>530</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="28" t="s">
         <v>646</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="28" t="s">
         <v>529</v>
       </c>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" t="s">
+      <c r="A82" s="28" t="s">
         <v>662</v>
       </c>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" t="s">
+      <c r="A83" s="28" t="s">
         <v>742</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="28" t="s">
         <v>686</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="28" t="s">
         <v>650</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="28" t="s">
         <v>650</v>
       </c>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" t="s">
+      <c r="A84" s="28" t="s">
         <v>750</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="28" t="s">
         <v>687</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="28" t="s">
         <v>651</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="28" t="s">
         <v>651</v>
       </c>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" t="s">
+      <c r="A85" s="28" t="s">
         <v>743</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="28" t="s">
         <v>688</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="28" t="s">
         <v>652</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D85" s="28" t="s">
         <v>652</v>
       </c>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" t="s">
+      <c r="A86" s="28" t="s">
         <v>744</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="28" t="s">
         <v>689</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="28" t="s">
         <v>653</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D86" s="28" t="s">
         <v>653</v>
       </c>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" t="s">
+      <c r="A87" s="28" t="s">
         <v>751</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="28" t="s">
         <v>690</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="28" t="s">
         <v>654</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="28" t="s">
         <v>654</v>
       </c>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" t="s">
+      <c r="A88" s="28" t="s">
         <v>745</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="28" t="s">
         <v>691</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="28" t="s">
         <v>655</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D88" s="28" t="s">
         <v>655</v>
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" t="s">
+      <c r="A89" s="28" t="s">
         <v>752</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="28" t="s">
         <v>692</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="28" t="s">
         <v>656</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="28" t="s">
         <v>656</v>
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" t="s">
+      <c r="A90" s="28" t="s">
         <v>746</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="28" t="s">
         <v>693</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="28" t="s">
         <v>657</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="28" t="s">
         <v>657</v>
       </c>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" t="s">
+      <c r="A91" s="28" t="s">
         <v>753</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="28" t="s">
         <v>694</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="28" t="s">
         <v>658</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="28" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" t="s">
+      <c r="A92" s="28" t="s">
         <v>747</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="28" t="s">
         <v>695</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="28" t="s">
         <v>659</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="28" t="s">
         <v>659</v>
       </c>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" t="s">
+      <c r="A93" s="28" t="s">
         <v>748</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="28" t="s">
         <v>696</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="28" t="s">
         <v>660</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="28" t="s">
         <v>660</v>
       </c>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" t="s">
+      <c r="A94" s="28" t="s">
         <v>749</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="28" t="s">
         <v>697</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C94" s="28" t="s">
         <v>661</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="28" t="s">
         <v>661</v>
       </c>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" t="s">
+      <c r="A95" s="28" t="s">
         <v>719</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="28" t="s">
         <v>698</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="28" t="s">
         <v>663</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="28" t="s">
         <v>663</v>
       </c>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" t="s">
+      <c r="A96" s="28" t="s">
         <v>720</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="28" t="s">
         <v>699</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="28" t="s">
         <v>664</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="28" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" t="s">
+      <c r="A97" s="28" t="s">
         <v>721</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="28" t="s">
         <v>700</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="28" t="s">
         <v>665</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="28" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" t="s">
+      <c r="A98" s="28" t="s">
         <v>722</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="28" t="s">
         <v>701</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="28" t="s">
         <v>666</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="28" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" t="s">
+      <c r="A99" s="28" t="s">
         <v>723</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="28" t="s">
         <v>702</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="28" t="s">
         <v>667</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D99" s="28" t="s">
         <v>667</v>
       </c>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" t="s">
+      <c r="A100" s="28" t="s">
         <v>724</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="28" t="s">
         <v>703</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="28" t="s">
         <v>668</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D100" s="28" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" t="s">
+      <c r="A101" s="28" t="s">
         <v>725</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="28" t="s">
         <v>704</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="28" t="s">
         <v>669</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="28" t="s">
         <v>669</v>
       </c>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" t="s">
+      <c r="A102" s="28" t="s">
         <v>726</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="28" t="s">
         <v>705</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="28" t="s">
         <v>670</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="28" t="s">
         <v>670</v>
       </c>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" t="s">
+      <c r="A103" s="28" t="s">
         <v>727</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="28" t="s">
         <v>706</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C103" s="28" t="s">
         <v>671</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D103" s="28" t="s">
         <v>671</v>
       </c>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" t="s">
+      <c r="A104" s="28" t="s">
         <v>728</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="28" t="s">
         <v>707</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C104" s="28" t="s">
         <v>672</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D104" s="28" t="s">
         <v>672</v>
       </c>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" t="s">
+      <c r="A105" s="28" t="s">
         <v>729</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="28" t="s">
         <v>708</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="28" t="s">
         <v>673</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="28" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" t="s">
+      <c r="A106" s="28" t="s">
         <v>730</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="28" t="s">
         <v>709</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="28" t="s">
         <v>674</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D106" s="28" t="s">
         <v>674</v>
       </c>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" t="s">
+      <c r="A107" s="28" t="s">
         <v>731</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="28" t="s">
         <v>710</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="28" t="s">
         <v>675</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D107" s="28" t="s">
         <v>675</v>
       </c>
     </row>
     <row r="108" spans="1:4">
-      <c r="A108" t="s">
+      <c r="A108" s="28" t="s">
         <v>732</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="28" t="s">
         <v>711</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="28" t="s">
         <v>676</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D108" s="28" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="109" spans="1:4">
-      <c r="A109" t="s">
+      <c r="A109" s="28" t="s">
         <v>733</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="28" t="s">
         <v>712</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="28" t="s">
         <v>677</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="28" t="s">
         <v>677</v>
       </c>
     </row>
     <row r="110" spans="1:4">
-      <c r="A110" t="s">
+      <c r="A110" s="28" t="s">
         <v>734</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="28" t="s">
         <v>713</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="28" t="s">
         <v>678</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D110" s="28" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="111" spans="1:4">
-      <c r="A111" t="s">
+      <c r="A111" s="28" t="s">
         <v>735</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="28" t="s">
         <v>714</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="28" t="s">
         <v>679</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="28" t="s">
         <v>679</v>
       </c>
     </row>
     <row r="112" spans="1:4">
-      <c r="A112" t="s">
+      <c r="A112" s="28" t="s">
         <v>736</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="28" t="s">
         <v>715</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="28" t="s">
         <v>680</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D112" s="28" t="s">
         <v>680</v>
       </c>
     </row>
     <row r="113" spans="1:4">
-      <c r="A113" t="s">
+      <c r="A113" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="28" t="s">
         <v>716</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="28" t="s">
         <v>681</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="28" t="s">
         <v>681</v>
       </c>
     </row>
     <row r="114" spans="1:4">
-      <c r="A114" t="s">
+      <c r="A114" s="28" t="s">
         <v>738</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="28" t="s">
         <v>717</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C114" s="28" t="s">
         <v>682</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D114" s="28" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="115" spans="1:4">
-      <c r="A115" t="s">
+      <c r="A115" s="28" t="s">
         <v>739</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="28" t="s">
         <v>718</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="28" t="s">
         <v>683</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D115" s="28" t="s">
         <v>683</v>
       </c>
     </row>
     <row r="116" spans="1:4">
-      <c r="A116" t="s">
+      <c r="A116" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="28" t="s">
         <v>807</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="28" t="s">
         <v>684</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="28" t="s">
         <v>684</v>
       </c>
     </row>
     <row r="117" spans="1:4">
-      <c r="A117" t="s">
+      <c r="A117" s="28" t="s">
         <v>741</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="28" t="s">
         <v>808</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="28" t="s">
         <v>685</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" s="28" t="s">
         <v>685</v>
       </c>
     </row>
     <row r="118" spans="1:4">
-      <c r="A118" t="s">
+      <c r="A118" s="28" t="s">
         <v>809</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="28" t="s">
         <v>849</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" s="28" t="s">
         <v>829</v>
       </c>
-      <c r="D118" t="s">
+      <c r="D118" s="28" t="s">
         <v>829</v>
       </c>
     </row>
     <row r="119" spans="1:4">
-      <c r="A119" t="s">
+      <c r="A119" s="28" t="s">
         <v>810</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="28" t="s">
         <v>850</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="28" t="s">
         <v>830</v>
       </c>
-      <c r="D119" t="s">
+      <c r="D119" s="28" t="s">
         <v>830</v>
       </c>
     </row>
     <row r="120" spans="1:4">
-      <c r="A120" t="s">
+      <c r="A120" s="28" t="s">
         <v>811</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="28" t="s">
         <v>851</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="28" t="s">
         <v>831</v>
       </c>
-      <c r="D120" t="s">
+      <c r="D120" s="28" t="s">
         <v>831</v>
       </c>
     </row>
     <row r="121" spans="1:4">
-      <c r="A121" t="s">
+      <c r="A121" s="28" t="s">
         <v>812</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="28" t="s">
         <v>852</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C121" s="28" t="s">
         <v>832</v>
       </c>
-      <c r="D121" t="s">
+      <c r="D121" s="28" t="s">
         <v>832</v>
       </c>
     </row>
     <row r="122" spans="1:4">
-      <c r="A122" t="s">
+      <c r="A122" s="28" t="s">
         <v>813</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="28" t="s">
         <v>853</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" s="28" t="s">
         <v>833</v>
       </c>
-      <c r="D122" t="s">
+      <c r="D122" s="28" t="s">
         <v>833</v>
       </c>
     </row>
     <row r="123" spans="1:4">
-      <c r="A123" t="s">
+      <c r="A123" s="28" t="s">
         <v>814</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="28" t="s">
         <v>854</v>
       </c>
-      <c r="C123" t="s">
+      <c r="C123" s="28" t="s">
         <v>834</v>
       </c>
-      <c r="D123" t="s">
+      <c r="D123" s="28" t="s">
         <v>834</v>
       </c>
     </row>
     <row r="124" spans="1:4">
-      <c r="A124" t="s">
+      <c r="A124" s="28" t="s">
         <v>815</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" s="28" t="s">
         <v>855</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C124" s="28" t="s">
         <v>835</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D124" s="28" t="s">
         <v>835</v>
       </c>
     </row>
     <row r="125" spans="1:4">
-      <c r="A125" t="s">
+      <c r="A125" s="28" t="s">
         <v>816</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="28" t="s">
         <v>856</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C125" s="28" t="s">
         <v>836</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D125" s="28" t="s">
         <v>836</v>
       </c>
     </row>
     <row r="126" spans="1:4">
-      <c r="A126" t="s">
+      <c r="A126" s="28" t="s">
         <v>817</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="28" t="s">
         <v>857</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C126" s="28" t="s">
         <v>837</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" s="28" t="s">
         <v>837</v>
       </c>
     </row>
     <row r="127" spans="1:4">
-      <c r="A127" t="s">
+      <c r="A127" s="28" t="s">
         <v>818</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="28" t="s">
         <v>858</v>
       </c>
-      <c r="C127" t="s">
+      <c r="C127" s="28" t="s">
         <v>838</v>
       </c>
-      <c r="D127" t="s">
+      <c r="D127" s="28" t="s">
         <v>838</v>
       </c>
     </row>
     <row r="128" spans="1:4">
-      <c r="A128" t="s">
+      <c r="A128" s="28" t="s">
         <v>819</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="28" t="s">
         <v>859</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C128" s="28" t="s">
         <v>839</v>
       </c>
-      <c r="D128" t="s">
+      <c r="D128" s="28" t="s">
         <v>839</v>
       </c>
     </row>
     <row r="129" spans="1:4">
-      <c r="A129" t="s">
+      <c r="A129" s="28" t="s">
         <v>820</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="28" t="s">
         <v>860</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="28" t="s">
         <v>840</v>
       </c>
-      <c r="D129" t="s">
+      <c r="D129" s="28" t="s">
         <v>840</v>
       </c>
     </row>
     <row r="130" spans="1:4">
-      <c r="A130" t="s">
+      <c r="A130" s="28" t="s">
         <v>821</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="28" t="s">
         <v>861</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C130" s="28" t="s">
         <v>841</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D130" s="28" t="s">
         <v>841</v>
       </c>
     </row>
     <row r="131" spans="1:4">
-      <c r="A131" t="s">
+      <c r="A131" s="28" t="s">
         <v>822</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="28" t="s">
         <v>862</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C131" s="28" t="s">
         <v>842</v>
       </c>
-      <c r="D131" t="s">
+      <c r="D131" s="28" t="s">
         <v>842</v>
       </c>
     </row>
     <row r="132" spans="1:4">
-      <c r="A132" t="s">
+      <c r="A132" s="28" t="s">
         <v>823</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="28" t="s">
         <v>863</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C132" s="28" t="s">
         <v>843</v>
       </c>
-      <c r="D132" t="s">
+      <c r="D132" s="28" t="s">
         <v>843</v>
       </c>
     </row>
     <row r="133" spans="1:4">
-      <c r="A133" t="s">
+      <c r="A133" s="28" t="s">
         <v>824</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="28" t="s">
         <v>864</v>
       </c>
-      <c r="C133" t="s">
+      <c r="C133" s="28" t="s">
         <v>844</v>
       </c>
-      <c r="D133" t="s">
+      <c r="D133" s="28" t="s">
         <v>844</v>
       </c>
     </row>
     <row r="134" spans="1:4">
-      <c r="A134" t="s">
+      <c r="A134" s="28" t="s">
         <v>825</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="28" t="s">
         <v>865</v>
       </c>
-      <c r="D134" t="s">
+      <c r="D134" s="28" t="s">
         <v>845</v>
       </c>
     </row>
     <row r="135" spans="1:4">
-      <c r="A135" t="s">
+      <c r="A135" s="28" t="s">
         <v>826</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="28" t="s">
         <v>866</v>
       </c>
-      <c r="D135" t="s">
+      <c r="D135" s="28" t="s">
         <v>846</v>
       </c>
     </row>
     <row r="136" spans="1:4">
-      <c r="A136" t="s">
+      <c r="A136" s="28" t="s">
         <v>827</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="28" t="s">
         <v>867</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D136" s="28" t="s">
         <v>847</v>
       </c>
     </row>
     <row r="137" spans="1:4">
-      <c r="A137" t="s">
+      <c r="A137" s="28" t="s">
         <v>828</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="28" t="s">
         <v>868</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D137" s="28" t="s">
         <v>848</v>
       </c>
     </row>
     <row r="138" spans="1:4">
-      <c r="A138" t="s">
+      <c r="A138" s="28" t="s">
         <v>870</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="28" t="s">
         <v>928</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C138" s="28" t="s">
         <v>877</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D138" s="28" t="s">
         <v>877</v>
       </c>
     </row>
     <row r="139" spans="1:4">
-      <c r="A139" t="s">
+      <c r="A139" s="28" t="s">
         <v>871</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="28" t="s">
         <v>929</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C139" s="28" t="s">
         <v>878</v>
       </c>
-      <c r="D139" t="s">
+      <c r="D139" s="28" t="s">
         <v>878</v>
       </c>
     </row>
     <row r="140" spans="1:4">
-      <c r="A140" t="s">
+      <c r="A140" s="28" t="s">
         <v>872</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="28" t="s">
         <v>930</v>
       </c>
-      <c r="C140" t="s">
+      <c r="C140" s="28" t="s">
         <v>879</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D140" s="28" t="s">
         <v>879</v>
       </c>
     </row>
     <row r="141" spans="1:4">
-      <c r="A141" t="s">
+      <c r="A141" s="28" t="s">
         <v>873</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="28" t="s">
         <v>931</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C141" s="28" t="s">
         <v>880</v>
       </c>
-      <c r="D141" t="s">
+      <c r="D141" s="28" t="s">
         <v>880</v>
       </c>
     </row>
-    <row r="142" spans="1:4" s="29" customFormat="1">
-      <c r="A142" s="29" t="s">
+    <row r="142" spans="1:4">
+      <c r="A142" s="28" t="s">
         <v>874</v>
       </c>
-      <c r="B142" s="29" t="s">
+      <c r="B142" s="28" t="s">
         <v>932</v>
       </c>
-      <c r="C142" s="29" t="s">
+      <c r="C142" s="28" t="s">
         <v>881</v>
       </c>
-      <c r="D142" s="29" t="s">
+      <c r="D142" s="28" t="s">
         <v>881</v>
       </c>
     </row>
     <row r="143" spans="1:4">
-      <c r="A143" t="s">
+      <c r="A143" s="28" t="s">
         <v>875</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="28" t="s">
         <v>933</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C143" s="28" t="s">
         <v>882</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D143" s="28" t="s">
         <v>882</v>
       </c>
     </row>
     <row r="144" spans="1:4">
-      <c r="A144" t="s">
+      <c r="A144" s="28" t="s">
         <v>876</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" s="28" t="s">
         <v>934</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C144" s="28" t="s">
         <v>883</v>
       </c>
-      <c r="D144" t="s">
+      <c r="D144" s="28" t="s">
         <v>883</v>
       </c>
     </row>
     <row r="145" spans="1:4">
-      <c r="A145" t="s">
+      <c r="A145" s="28" t="s">
         <v>892</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B145" s="28" t="s">
         <v>935</v>
       </c>
-      <c r="D145" t="s">
+      <c r="D145" s="28" t="s">
         <v>893</v>
       </c>
     </row>
     <row r="146" spans="1:4">
-      <c r="A146" t="s">
+      <c r="A146" s="28" t="s">
         <v>884</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="28" t="s">
         <v>936</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D146" s="28" t="s">
         <v>885</v>
       </c>
     </row>
-    <row r="147" spans="1:4" s="28" customFormat="1">
+    <row r="147" spans="1:4">
       <c r="A147" s="28" t="s">
         <v>889</v>
       </c>
@@ -11293,70 +11394,70 @@
       </c>
     </row>
     <row r="148" spans="1:4">
-      <c r="A148" t="s">
+      <c r="A148" s="28" t="s">
         <v>891</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="28" t="s">
         <v>916</v>
       </c>
     </row>
     <row r="149" spans="1:4">
-      <c r="A149" t="s">
+      <c r="A149" s="28" t="s">
         <v>918</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="28" t="s">
         <v>915</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D149" s="28" t="s">
         <v>917</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="29">
-      <c r="A150" s="5" t="s">
+      <c r="A150" s="29" t="s">
         <v>919</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B150" s="28" t="s">
         <v>924</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D150" s="28" t="s">
         <v>938</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="43.5">
-      <c r="A151" s="5" t="s">
+      <c r="A151" s="29" t="s">
         <v>920</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B151" s="28" t="s">
         <v>925</v>
       </c>
-      <c r="D151" t="s">
+      <c r="D151" s="28" t="s">
         <v>939</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="29">
-      <c r="A152" s="5" t="s">
+      <c r="A152" s="29" t="s">
         <v>921</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B152" s="28" t="s">
         <v>926</v>
       </c>
-      <c r="D152" t="s">
+      <c r="D152" s="28" t="s">
         <v>940</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="29">
-      <c r="A153" s="5" t="s">
+      <c r="A153" s="29" t="s">
         <v>922</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B153" s="28" t="s">
         <v>927</v>
       </c>
-      <c r="D153" t="s">
+      <c r="D153" s="28" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="154" spans="1:4" s="28" customFormat="1" ht="29">
-      <c r="A154" s="30" t="s">
+    <row r="154" spans="1:4" ht="29">
+      <c r="A154" s="29" t="s">
         <v>923</v>
       </c>
       <c r="B154" s="28" t="s">
@@ -11366,18 +11467,18 @@
         <v>942</v>
       </c>
     </row>
-    <row r="155" spans="1:4" s="29" customFormat="1" ht="29">
-      <c r="A155" s="31" t="s">
+    <row r="155" spans="1:4" ht="29">
+      <c r="A155" s="29" t="s">
         <v>894</v>
       </c>
-      <c r="B155" s="29" t="s">
+      <c r="B155" s="28" t="s">
         <v>897</v>
       </c>
-      <c r="D155" s="29" t="s">
+      <c r="D155" s="28" t="s">
         <v>898</v>
       </c>
     </row>
-    <row r="156" spans="1:4" s="28" customFormat="1">
+    <row r="156" spans="1:4">
       <c r="A156" s="28" t="s">
         <v>895</v>
       </c>
@@ -11388,62 +11489,62 @@
         <v>902</v>
       </c>
     </row>
-    <row r="157" spans="1:4" s="29" customFormat="1">
-      <c r="A157" s="29" t="s">
+    <row r="157" spans="1:4">
+      <c r="A157" s="28" t="s">
         <v>896</v>
       </c>
-      <c r="B157" s="29" t="s">
+      <c r="B157" s="28" t="s">
         <v>900</v>
       </c>
-      <c r="D157" s="29" t="s">
+      <c r="D157" s="28" t="s">
         <v>901</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="29">
-      <c r="A158" s="5" t="s">
+      <c r="A158" s="29" t="s">
         <v>903</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="28" t="s">
         <v>914</v>
       </c>
-      <c r="D158" t="s">
+      <c r="D158" s="28" t="s">
         <v>904</v>
       </c>
     </row>
     <row r="159" spans="1:4">
-      <c r="A159" t="s">
+      <c r="A159" s="28" t="s">
         <v>906</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="28" t="s">
         <v>913</v>
       </c>
-      <c r="D159" t="s">
+      <c r="D159" s="28" t="s">
         <v>905</v>
       </c>
     </row>
     <row r="160" spans="1:4">
-      <c r="A160" t="s">
+      <c r="A160" s="28" t="s">
         <v>907</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="28" t="s">
         <v>911</v>
       </c>
-      <c r="D160" t="s">
+      <c r="D160" s="28" t="s">
         <v>908</v>
       </c>
     </row>
     <row r="161" spans="1:4">
-      <c r="A161" t="s">
+      <c r="A161" s="28" t="s">
         <v>910</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="28" t="s">
         <v>912</v>
       </c>
-      <c r="D161" t="s">
+      <c r="D161" s="28" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="162" spans="1:4" s="28" customFormat="1">
+    <row r="162" spans="1:4">
       <c r="A162" s="28" t="s">
         <v>944</v>
       </c>
@@ -11457,7 +11558,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="163" spans="1:4" s="28" customFormat="1">
+    <row r="163" spans="1:4">
       <c r="A163" s="28" t="s">
         <v>948</v>
       </c>
@@ -11471,39 +11572,95 @@
         <v>946</v>
       </c>
     </row>
+    <row r="164" spans="1:4">
+      <c r="A164" s="28" t="s">
+        <v>2294</v>
+      </c>
+      <c r="B164" s="28" t="s">
+        <v>2276</v>
+      </c>
+      <c r="D164" s="28" t="s">
+        <v>2283</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" s="28" t="s">
+        <v>2284</v>
+      </c>
+      <c r="B165" s="28" t="s">
+        <v>2273</v>
+      </c>
+      <c r="D165" s="28" t="s">
+        <v>2285</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" t="s">
+        <v>2286</v>
+      </c>
+      <c r="B166" s="28" t="s">
+        <v>2277</v>
+      </c>
+      <c r="D166" s="28" t="s">
+        <v>2287</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="28" t="s">
+        <v>2288</v>
+      </c>
+      <c r="B167" s="28" t="s">
+        <v>2290</v>
+      </c>
+      <c r="D167" s="28" t="s">
+        <v>2289</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" s="28" t="s">
+        <v>2291</v>
+      </c>
+      <c r="B168" s="28" t="s">
+        <v>2292</v>
+      </c>
+      <c r="D168" s="28" t="s">
+        <v>2293</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B83:B163">
-    <cfRule type="duplicateValues" dxfId="12" priority="17"/>
-  </conditionalFormatting>
+  <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="C1:C82 C118:C1048576 D53:D54">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D118:D137">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D138">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D139">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D141">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D142">
-    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D143">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D144">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D162:D163">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83:B169">
+    <cfRule type="duplicateValues" dxfId="2" priority="18"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11511,13 +11668,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C79ADD9-972D-451E-A958-4DB073B90EB6}">
-  <dimension ref="A1:M122"/>
+  <dimension ref="A1:M130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I113" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B122" sqref="B122"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -13080,6 +13237,94 @@
       </c>
       <c r="M122" s="28" t="s">
         <v>2254</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" s="28" customFormat="1">
+      <c r="A123" s="28" t="s">
+        <v>2259</v>
+      </c>
+      <c r="B123" s="28" t="s">
+        <v>2273</v>
+      </c>
+      <c r="E123" s="28" t="s">
+        <v>2260</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" s="28" customFormat="1">
+      <c r="A124" s="28" t="s">
+        <v>2261</v>
+      </c>
+      <c r="B124" s="28" t="s">
+        <v>2274</v>
+      </c>
+      <c r="E124" s="28" t="s">
+        <v>2262</v>
+      </c>
+    </row>
+    <row r="125" spans="1:13">
+      <c r="A125" t="s">
+        <v>2263</v>
+      </c>
+      <c r="B125" s="28" t="s">
+        <v>2275</v>
+      </c>
+      <c r="E125" t="s">
+        <v>2264</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13">
+      <c r="A126" t="s">
+        <v>2265</v>
+      </c>
+      <c r="B126" s="28" t="s">
+        <v>2276</v>
+      </c>
+      <c r="E126" t="s">
+        <v>2266</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13">
+      <c r="A127" t="s">
+        <v>2267</v>
+      </c>
+      <c r="B127" s="28" t="s">
+        <v>2277</v>
+      </c>
+      <c r="E127" t="s">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="128" spans="1:13">
+      <c r="A128" t="s">
+        <v>2269</v>
+      </c>
+      <c r="B128" s="28" t="s">
+        <v>2278</v>
+      </c>
+      <c r="E128" t="s">
+        <v>2270</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" t="s">
+        <v>2271</v>
+      </c>
+      <c r="B129" s="28" t="s">
+        <v>2279</v>
+      </c>
+      <c r="E129" t="s">
+        <v>2272</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" t="s">
+        <v>2280</v>
+      </c>
+      <c r="B130" s="28" t="s">
+        <v>2282</v>
+      </c>
+      <c r="E130" t="s">
+        <v>2281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>